<commit_message>
02.09.19 Toady Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 01.09.19</t>
+    <t>Date: 02.09.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+      <selection activeCell="K47" sqref="A1:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>40</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>28</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>40000</v>
+        <v>28000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>159</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>52</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>79500</v>
+        <v>26000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>291</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>360</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>29100</v>
+        <v>36000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>148</v>
-      </c>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,8 +3009,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3028,8 +3026,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3042,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>156000</v>
+        <v>90000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3092,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3153,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3242,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3304,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3322,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>40</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>28</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>40000</v>
+        <v>28000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3341,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>159</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>52</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>79500</v>
+        <v>26000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3360,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>291</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>360</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>29100</v>
+        <v>36000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3379,13 +3377,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <v>148</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3398,8 +3394,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3415,8 +3411,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3429,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>156000</v>
+        <v>90000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3479,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3540,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3570,28 +3566,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3608,6 +3582,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3638,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3704,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3722,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3741,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3760,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3779,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3881,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4025,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4087,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4105,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4124,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4143,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4162,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4214,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4264,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4361,30 +4357,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4401,6 +4373,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4432,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4498,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4516,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4535,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4554,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4573,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4590,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4607,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4621,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4671,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4811,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4873,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4891,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4910,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4929,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4948,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4965,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4982,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4996,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5046,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5139,6 +5135,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5151,34 +5175,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5203,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5271,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5283,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5295,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5307,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5319,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5331,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5342,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5387,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5442,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5531,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5595,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5613,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5632,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5651,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5670,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5687,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5704,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5770,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5831,20 +5827,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5857,24 +5863,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5900,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6081,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6099,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6116,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6135,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6152,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6171,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6188,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6254,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6315,29 +6311,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6354,6 +6333,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
03.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 02.09.19</t>
+    <t>Date: 03.09.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="A1:K47"/>
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>28</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>23</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>28000</v>
+        <v>23000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>52</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>67</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>26000</v>
+        <v>33500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>360</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>415</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>36000</v>
+        <v>41500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,8 +2992,8 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3009,8 +3009,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3026,8 +3026,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3040,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>90000</v>
+        <v>98000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>28</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>23</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>28000</v>
+        <v>23000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>52</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>67</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>26000</v>
+        <v>33500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>360</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>415</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>36000</v>
+        <v>41500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,8 +3377,8 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3394,8 +3394,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3411,8 +3411,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3425,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>90000</v>
+        <v>98000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,6 +3566,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3582,28 +3604,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,6 +4357,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4373,30 +4397,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,16 +5135,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5157,24 +5165,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,12 +5827,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5845,32 +5871,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,12 +6311,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6333,23 +6350,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
04.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 03.09.19</t>
+    <t>Date: 04.09.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>23</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>52</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>23000</v>
+        <v>52000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>67</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>72</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>33500</v>
+        <v>36000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>415</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>47</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>41500</v>
+        <v>4700</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,11 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44">
+        <v>126</v>
+      </c>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6300</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3009,11 +3011,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44">
+        <v>80</v>
+      </c>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3026,11 +3030,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44">
+        <v>240</v>
+      </c>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3040,14 +3046,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>98000</v>
+        <v>103000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3096,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3157,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3246,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3308,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3326,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>23</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>52</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>23000</v>
+        <v>52000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3345,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>67</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>72</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>33500</v>
+        <v>36000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3364,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>415</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>47</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>41500</v>
+        <v>4700</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,11 +3383,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44">
+        <v>126</v>
+      </c>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6300</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3394,11 +3402,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44">
+        <v>80</v>
+      </c>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3411,11 +3421,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44">
+        <v>240</v>
+      </c>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3425,14 +3437,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>98000</v>
+        <v>103000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3487,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3548,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,28 +3578,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3604,6 +3594,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3646,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3712,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3730,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3749,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3768,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3787,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3806,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3825,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3839,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3889,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4033,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4095,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4113,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4132,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4151,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4170,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4189,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4208,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4222,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4272,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,30 +4369,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4397,6 +4385,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4440,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4506,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4524,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4543,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4562,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4581,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4598,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4615,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4629,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4679,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4819,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4881,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4899,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4918,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4937,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4956,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4973,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4990,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +5004,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5054,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,6 +5147,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5147,34 +5187,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5211,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5279,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5291,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5303,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5315,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5327,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5339,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5350,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5395,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5450,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5539,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5603,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5621,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5640,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5659,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5678,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5695,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5712,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5778,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,20 +5839,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5853,24 +5875,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5908,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6089,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6107,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6124,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6143,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6160,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6179,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6196,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6262,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,29 +6323,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6350,6 +6345,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
05.09.19 Todoy Sales Updated
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 04.09.19</t>
+    <t>Date: 05.09.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>52</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>67</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>52000</v>
+        <v>67000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>72</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>89</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>36000</v>
+        <v>44500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>47</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>388</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>38800</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>126</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54">
+        <v>114</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>6300</v>
+        <v>5700</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,13 +3011,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>80</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3030,13 +3028,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44">
-        <v>240</v>
-      </c>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>2400</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3046,14 +3042,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>103000</v>
+        <v>156000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3096,58 +3092,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3157,9 +3153,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3246,60 +3242,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3308,10 +3304,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3326,13 +3322,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>52</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>67</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>52000</v>
+        <v>67000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3345,13 +3341,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>72</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>89</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>36000</v>
+        <v>44500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3364,13 +3360,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>47</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>388</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>4700</v>
+        <v>38800</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3383,13 +3379,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>126</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54">
+        <v>114</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>6300</v>
+        <v>5700</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3402,13 +3398,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>80</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3421,13 +3415,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44">
-        <v>240</v>
-      </c>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>2400</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3437,14 +3429,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>103000</v>
+        <v>156000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3487,58 +3479,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3548,9 +3540,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3578,6 +3570,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3594,28 +3608,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3646,63 +3638,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3712,10 +3704,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3730,10 +3722,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3749,10 +3741,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3768,10 +3760,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3787,10 +3779,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3806,10 +3798,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3825,8 +3817,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3839,10 +3831,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3889,76 +3881,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4033,60 +4025,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4095,10 +4087,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4113,10 +4105,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4132,10 +4124,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4151,10 +4143,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4170,10 +4162,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4189,10 +4181,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4208,8 +4200,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4222,10 +4214,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4272,76 +4264,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4369,6 +4361,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4385,30 +4401,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4440,63 +4432,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4506,10 +4498,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4524,10 +4516,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4543,10 +4535,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4562,10 +4554,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4581,8 +4573,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4598,8 +4590,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4615,8 +4607,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4629,10 +4621,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4679,72 +4671,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4819,60 +4811,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4881,10 +4873,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4899,10 +4891,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4918,10 +4910,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4937,10 +4929,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4956,8 +4948,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4973,8 +4965,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4990,8 +4982,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5004,10 +4996,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5054,72 +5046,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5147,16 +5139,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5169,24 +5169,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5211,64 +5203,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5279,8 +5271,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5291,8 +5283,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5303,8 +5295,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5315,8 +5307,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5327,8 +5319,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5339,8 +5331,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5350,8 +5342,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5395,52 +5387,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5450,9 +5442,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5539,60 +5531,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5603,10 +5595,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5621,10 +5613,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5640,10 +5632,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5659,10 +5651,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5678,8 +5670,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5695,8 +5687,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5712,10 +5704,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5778,58 +5770,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5839,12 +5831,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5857,32 +5875,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5908,177 +5900,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6089,10 +6081,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6107,8 +6099,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6124,10 +6116,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6143,8 +6135,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6160,10 +6152,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6179,8 +6171,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6196,10 +6188,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6262,58 +6254,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6323,12 +6315,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6345,23 +6354,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
08.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 07.09.19</t>
+    <t>Date: 08.09.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>51</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>42</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>51000</v>
+        <v>42000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>120</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>100</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>281</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>200</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>28100</v>
+        <v>20000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>41</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>2050</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,13 +3009,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>5</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3030,13 +3026,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44">
-        <v>175</v>
-      </c>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3046,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>143000</v>
+        <v>112000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3096,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3157,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3246,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3308,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3326,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>51</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>42</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>51000</v>
+        <v>42000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3345,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>120</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>100</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3364,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>281</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>200</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>28100</v>
+        <v>20000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3383,13 +3377,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>41</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>2050</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3402,13 +3394,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>5</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3421,13 +3411,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44">
-        <v>175</v>
-      </c>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3437,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>143000</v>
+        <v>112000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3487,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3548,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3578,6 +3566,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3594,28 +3604,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3646,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3712,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3730,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3749,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3768,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3787,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3806,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3825,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3839,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3889,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4033,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4095,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4113,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4132,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4151,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4170,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4189,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4208,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4222,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4272,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4369,6 +4357,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4385,30 +4397,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4440,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4506,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4524,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4543,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4562,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4581,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4598,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4615,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4629,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4679,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4819,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4881,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4899,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4918,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4937,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4956,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4973,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4990,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5004,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5054,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5147,16 +5135,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5169,24 +5165,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5211,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5279,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5291,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5303,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5315,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5327,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5339,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5350,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5395,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5450,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5539,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5603,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5621,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5640,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5659,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5678,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5695,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5712,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5778,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5839,12 +5827,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5857,32 +5871,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5908,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6089,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6107,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6124,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6143,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6160,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6179,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6196,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6262,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6323,12 +6311,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6345,23 +6350,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
09.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -101,7 +101,10 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 08.09.19</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Date: 09.09.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +476,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +548,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +569,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +582,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +609,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2079,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2141,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2159,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2178,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2197,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2216,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2235,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2252,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2266,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2316,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2377,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2456,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2518,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2536,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2555,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2574,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2593,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2612,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2629,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2643,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2693,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2754,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2786,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2816,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,8 +2835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H44" sqref="A1:J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2854,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="A4" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2920,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2938,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>42</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>23</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>42000</v>
+        <v>23000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2957,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>100</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>177</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>88500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2976,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>200</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>96</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>9600</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,11 +2995,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44">
+        <v>5</v>
+      </c>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3009,11 +3014,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44">
+        <v>25</v>
+      </c>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3026,11 +3033,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44">
+        <v>15</v>
+      </c>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3040,14 +3049,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>112000</v>
+        <v>122000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3099,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3160,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3249,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="A31" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3311,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3329,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>42</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>23</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>42000</v>
+        <v>23000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3348,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>100</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>177</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>88500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3367,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>200</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>96</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>9600</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,11 +3386,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44">
+        <v>5</v>
+      </c>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3394,11 +3405,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44">
+        <v>25</v>
+      </c>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3411,11 +3424,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44">
+        <v>15</v>
+      </c>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3425,14 +3440,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>112000</v>
+        <v>122000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3490,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="H46" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3551,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,28 +3581,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3604,6 +3597,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3649,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3715,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3733,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3752,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3771,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3790,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3809,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3828,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3842,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3892,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4036,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4098,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4116,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4135,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4154,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4173,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4192,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4211,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4225,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4275,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,30 +4372,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4397,6 +4388,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4443,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4509,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4527,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4546,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4565,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4584,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4601,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4618,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4632,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4682,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4822,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4884,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4902,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4921,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4940,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4959,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4976,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4993,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +5007,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5057,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,6 +5150,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5147,34 +5190,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5214,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5282,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5294,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5306,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5318,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5330,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5342,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5353,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5398,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5453,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5542,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5606,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5624,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5643,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5662,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5681,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5698,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5715,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5781,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,20 +5842,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5853,24 +5878,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5911,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6092,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6110,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6127,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6146,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6163,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6182,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6199,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6265,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,29 +6326,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6350,6 +6348,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
11.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Date: 10.09.19</t>
+    <t>Date: 11.09.19</t>
   </si>
 </sst>
 </file>
@@ -476,47 +476,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,34 +548,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -566,15 +569,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -582,6 +582,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -603,12 +609,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2057,7 +2057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2079,60 +2079,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2141,10 +2141,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2159,10 +2159,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2178,10 +2178,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2197,10 +2197,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2216,10 +2216,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2235,8 +2235,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2252,8 +2252,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2266,10 +2266,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2316,58 +2316,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2377,11 +2377,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2456,60 +2456,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2518,10 +2518,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2536,10 +2536,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2555,10 +2555,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2574,10 +2574,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2593,10 +2593,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2612,8 +2612,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2629,8 +2629,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2643,10 +2643,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2693,58 +2693,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2754,11 +2754,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2786,14 +2786,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2806,24 +2816,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2854,63 +2854,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2920,10 +2920,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2938,13 +2938,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>50</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>33</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>50000</v>
+        <v>33000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2957,13 +2957,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>60</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>146</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>73000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>100</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>244</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>24400</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2995,11 +2995,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44">
+        <v>144</v>
+      </c>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7200</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3012,11 +3014,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44">
+        <v>63</v>
+      </c>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3029,11 +3033,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44">
+        <v>14</v>
+      </c>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3043,14 +3049,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>90000</v>
+        <v>139000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3093,58 +3099,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3154,9 +3160,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3243,60 +3249,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3305,10 +3311,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3323,13 +3329,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>50</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>33</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>50000</v>
+        <v>33000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3342,13 +3348,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>60</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>146</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>73000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3361,13 +3367,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>100</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>244</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>24400</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3380,11 +3386,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44">
+        <v>144</v>
+      </c>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7200</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3397,11 +3405,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44">
+        <v>63</v>
+      </c>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3414,11 +3424,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44">
+        <v>14</v>
+      </c>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3428,14 +3440,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>90000</v>
+        <v>139000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3478,58 +3490,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3539,9 +3551,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3569,28 +3581,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3607,6 +3597,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3637,63 +3649,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3703,10 +3715,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3721,10 +3733,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3740,10 +3752,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3759,10 +3771,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3778,10 +3790,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3797,10 +3809,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3816,8 +3828,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3830,10 +3842,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3880,76 +3892,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4024,60 +4036,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4086,10 +4098,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4104,10 +4116,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4123,10 +4135,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4142,10 +4154,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4161,10 +4173,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4180,10 +4192,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4199,8 +4211,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4213,10 +4225,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4263,76 +4275,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4360,30 +4372,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4400,6 +4388,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4431,63 +4443,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4497,10 +4509,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4515,10 +4527,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4534,10 +4546,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4553,10 +4565,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4572,8 +4584,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4589,8 +4601,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4606,8 +4618,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4620,10 +4632,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4670,72 +4682,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4810,60 +4822,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4872,10 +4884,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4890,10 +4902,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4909,10 +4921,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4928,10 +4940,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4947,8 +4959,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4964,8 +4976,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4981,8 +4993,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4995,10 +5007,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5045,72 +5057,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5138,6 +5150,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5150,34 +5190,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5202,64 +5214,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5270,8 +5282,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5282,8 +5294,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5294,8 +5306,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5306,8 +5318,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5318,8 +5330,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5330,8 +5342,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5341,8 +5353,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5386,52 +5398,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5441,9 +5453,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5530,60 +5542,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5594,10 +5606,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5612,10 +5624,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5631,10 +5643,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5650,10 +5662,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5669,8 +5681,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5686,8 +5698,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5703,10 +5715,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5769,58 +5781,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5830,20 +5842,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5856,24 +5878,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5899,177 +5911,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6080,10 +6092,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6098,8 +6110,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6115,10 +6127,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6134,8 +6146,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6151,10 +6163,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6170,8 +6182,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6187,10 +6199,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6253,58 +6265,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6314,29 +6326,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6353,6 +6348,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
12.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Date: 11.09.19</t>
+    <t>Date: 12.09.19</t>
   </si>
 </sst>
 </file>
@@ -2939,12 +2939,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="44">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>33000</v>
+        <v>19000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2958,12 +2958,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="44">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>73000</v>
+        <v>59500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2977,12 +2977,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="44">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>24400</v>
+        <v>20000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2996,12 +2996,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="44">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>7200</v>
+        <v>50</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3015,12 +3015,12 @@
         <v>20</v>
       </c>
       <c r="E10" s="44">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>1260</v>
+        <v>2200</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3034,12 +3034,12 @@
         <v>10</v>
       </c>
       <c r="E11" s="44">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3056,7 +3056,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>139000</v>
+        <v>101000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3330,12 +3330,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="44">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>33000</v>
+        <v>19000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3349,12 +3349,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="44">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>73000</v>
+        <v>59500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3368,12 +3368,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="44">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>24400</v>
+        <v>20000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3387,12 +3387,12 @@
         <v>50</v>
       </c>
       <c r="E36" s="44">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>7200</v>
+        <v>50</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3406,12 +3406,12 @@
         <v>20</v>
       </c>
       <c r="E37" s="44">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>1260</v>
+        <v>2200</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3425,12 +3425,12 @@
         <v>10</v>
       </c>
       <c r="E38" s="44">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3447,7 +3447,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>139000</v>
+        <v>101000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
14.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Date: 12.09.19</t>
+    <t>Date: 14.09.19</t>
   </si>
 </sst>
 </file>
@@ -476,12 +476,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -491,90 +518,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -582,12 +582,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -609,6 +603,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2057,7 +2057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2079,60 +2079,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2141,10 +2141,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2159,10 +2159,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2178,10 +2178,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2197,10 +2197,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2216,10 +2216,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2235,8 +2235,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2252,8 +2252,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2266,10 +2266,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2316,58 +2316,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2377,11 +2377,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2456,60 +2456,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2518,10 +2518,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2536,10 +2536,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2555,10 +2555,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2574,10 +2574,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2593,10 +2593,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2612,8 +2612,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2629,8 +2629,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2643,10 +2643,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2693,58 +2693,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2754,11 +2754,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2786,6 +2786,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2798,32 +2824,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2835,7 +2835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection sqref="A1:J45"/>
     </sheetView>
   </sheetViews>
@@ -2854,63 +2854,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2920,10 +2920,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2938,13 +2938,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>19</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>47</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>19000</v>
+        <v>47000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2957,13 +2957,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>119</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>150</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>59500</v>
+        <v>75000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>200</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>310</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>31000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>1</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54">
+        <v>10</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>110</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54">
+        <v>25</v>
+      </c>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2200</v>
+        <v>500</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44">
-        <v>25</v>
-      </c>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54">
+        <v>300</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>3000</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3049,14 +3049,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>101000</v>
+        <v>157000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3099,58 +3099,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3160,9 +3160,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3249,60 +3249,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3311,10 +3311,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3329,13 +3329,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>19</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>47</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>19000</v>
+        <v>47000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3348,13 +3348,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>119</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>150</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>59500</v>
+        <v>75000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3367,13 +3367,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>200</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>310</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>31000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3386,13 +3386,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>1</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54">
+        <v>10</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3405,13 +3405,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>110</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54">
+        <v>25</v>
+      </c>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2200</v>
+        <v>500</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3424,13 +3424,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44">
-        <v>25</v>
-      </c>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54">
+        <v>300</v>
+      </c>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>3000</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3440,14 +3440,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>101000</v>
+        <v>157000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3490,58 +3490,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3551,9 +3551,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3581,6 +3581,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3597,28 +3619,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3649,63 +3649,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3715,10 +3715,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3733,10 +3733,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3752,10 +3752,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3771,10 +3771,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3790,10 +3790,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3809,10 +3809,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3828,8 +3828,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3842,10 +3842,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3892,76 +3892,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4036,60 +4036,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4098,10 +4098,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4116,10 +4116,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4135,10 +4135,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4154,10 +4154,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4173,10 +4173,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4192,10 +4192,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4211,8 +4211,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4225,10 +4225,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4275,76 +4275,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4372,6 +4372,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4388,30 +4412,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4443,63 +4443,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4509,10 +4509,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4527,10 +4527,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4546,10 +4546,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4565,10 +4565,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4584,8 +4584,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4601,8 +4601,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4618,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4632,10 +4632,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4682,72 +4682,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4822,60 +4822,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4884,10 +4884,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4902,10 +4902,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4921,10 +4921,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4940,10 +4940,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4959,8 +4959,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4976,8 +4976,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4993,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5007,10 +5007,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5057,72 +5057,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5150,16 +5150,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5172,24 +5180,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5214,64 +5214,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5282,8 +5282,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5294,8 +5294,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5306,8 +5306,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5318,8 +5318,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5330,8 +5330,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5342,8 +5342,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5353,8 +5353,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5398,52 +5398,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5453,9 +5453,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5542,60 +5542,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5606,10 +5606,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5624,10 +5624,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5643,10 +5643,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5662,10 +5662,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5681,8 +5681,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5698,8 +5698,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5715,10 +5715,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5781,58 +5781,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5842,12 +5842,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5860,32 +5886,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5911,177 +5911,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6092,10 +6092,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6110,8 +6110,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6127,10 +6127,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6146,8 +6146,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6163,10 +6163,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6182,8 +6182,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6199,10 +6199,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6265,58 +6265,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6326,12 +6326,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6348,23 +6365,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
15.09.19 Today Sales details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Date: 14.09.19</t>
+    <t>Date: 15.09.19</t>
   </si>
 </sst>
 </file>
@@ -2835,7 +2835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J45"/>
     </sheetView>
   </sheetViews>
@@ -2939,12 +2939,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="54">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>47000</v>
+        <v>22000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2958,12 +2958,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="54">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>75000</v>
+        <v>77500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2977,12 +2977,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="54">
-        <v>310</v>
+        <v>169</v>
       </c>
       <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>31000</v>
+        <v>16900</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2996,12 +2996,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="54">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>2600</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3014,13 +3014,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54">
-        <v>25</v>
-      </c>
+      <c r="E10" s="54"/>
       <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3033,13 +3031,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54">
-        <v>300</v>
-      </c>
+      <c r="E11" s="54"/>
       <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3056,7 +3052,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>157000</v>
+        <v>119000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3330,12 +3326,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="54">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>47000</v>
+        <v>22000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3349,12 +3345,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="54">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>75000</v>
+        <v>77500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3368,12 +3364,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="54">
-        <v>310</v>
+        <v>169</v>
       </c>
       <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>31000</v>
+        <v>16900</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3387,12 +3383,12 @@
         <v>50</v>
       </c>
       <c r="E36" s="54">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>2600</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3405,13 +3401,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54">
-        <v>25</v>
-      </c>
+      <c r="E37" s="54"/>
       <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3424,13 +3418,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54">
-        <v>300</v>
-      </c>
+      <c r="E38" s="54"/>
       <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3447,7 +3439,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>157000</v>
+        <v>119000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
16.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Date: 15.09.19</t>
+    <t>Date: 16.09.19</t>
   </si>
 </sst>
 </file>
@@ -476,47 +476,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,34 +548,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -566,15 +569,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -582,6 +582,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -603,12 +609,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2057,7 +2057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2079,60 +2079,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2141,10 +2141,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2159,10 +2159,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2178,10 +2178,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2197,10 +2197,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2216,10 +2216,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2235,8 +2235,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2252,8 +2252,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2266,10 +2266,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2316,58 +2316,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2377,11 +2377,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2456,60 +2456,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2518,10 +2518,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2536,10 +2536,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2555,10 +2555,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2574,10 +2574,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2593,10 +2593,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2612,8 +2612,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2629,8 +2629,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2643,10 +2643,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2693,58 +2693,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2754,11 +2754,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2786,14 +2786,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2806,24 +2816,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2835,7 +2835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
       <selection sqref="A1:J45"/>
     </sheetView>
   </sheetViews>
@@ -2854,63 +2854,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2920,10 +2920,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2938,13 +2938,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>22</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>64</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>22000</v>
+        <v>64000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2957,13 +2957,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>155</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>132</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>77500</v>
+        <v>66000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>169</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>81</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>16900</v>
+        <v>8100</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2995,13 +2995,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>52</v>
-      </c>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>2600</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3014,8 +3012,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3031,11 +3029,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44">
+        <v>190</v>
+      </c>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1900</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3045,14 +3045,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>119000</v>
+        <v>140000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3095,58 +3095,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3156,9 +3156,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3245,60 +3245,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3307,10 +3307,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3325,13 +3325,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>22</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>64</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>22000</v>
+        <v>64000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3344,13 +3344,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>155</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>132</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>77500</v>
+        <v>66000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3363,13 +3363,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>169</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>81</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>16900</v>
+        <v>8100</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3382,13 +3382,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <v>52</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>2600</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3401,8 +3399,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3418,11 +3416,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44">
+        <v>190</v>
+      </c>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1900</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3432,14 +3432,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>119000</v>
+        <v>140000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3482,58 +3482,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3543,9 +3543,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3573,28 +3573,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3611,6 +3589,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3641,63 +3641,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3707,10 +3707,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3725,10 +3725,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3744,10 +3744,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3763,10 +3763,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3782,10 +3782,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3801,10 +3801,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3820,8 +3820,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3834,10 +3834,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3884,76 +3884,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4028,60 +4028,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4090,10 +4090,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4108,10 +4108,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4127,10 +4127,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4146,10 +4146,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4165,10 +4165,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4184,10 +4184,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4203,8 +4203,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4217,10 +4217,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4267,76 +4267,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4364,30 +4364,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4404,6 +4380,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4435,63 +4435,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4501,10 +4501,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4519,10 +4519,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4538,10 +4538,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4557,10 +4557,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4576,8 +4576,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4593,8 +4593,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4610,8 +4610,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4624,10 +4624,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4674,72 +4674,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4814,60 +4814,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4876,10 +4876,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4894,10 +4894,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4913,10 +4913,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4932,10 +4932,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4951,8 +4951,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4968,8 +4968,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4985,8 +4985,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4999,10 +4999,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5049,72 +5049,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5142,6 +5142,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5154,34 +5182,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5206,64 +5206,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5274,8 +5274,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5286,8 +5286,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5298,8 +5298,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5310,8 +5310,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5322,8 +5322,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5334,8 +5334,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5345,8 +5345,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5390,52 +5390,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5445,9 +5445,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5534,60 +5534,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5598,10 +5598,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5616,10 +5616,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5635,10 +5635,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5654,10 +5654,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5673,8 +5673,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5690,8 +5690,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5707,10 +5707,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5773,58 +5773,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5834,20 +5834,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5860,24 +5870,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5903,177 +5903,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6084,10 +6084,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6102,8 +6102,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6119,10 +6119,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6138,8 +6138,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6155,10 +6155,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6174,8 +6174,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6191,10 +6191,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6257,58 +6257,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6318,29 +6318,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6357,6 +6340,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
17.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Date: 16.09.19</t>
+    <t>Date: 17.09.19</t>
   </si>
 </sst>
 </file>
@@ -2939,12 +2939,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="44">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>64000</v>
+        <v>42000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2958,12 +2958,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="44">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>66000</v>
+        <v>75500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2977,12 +2977,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="44">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>8100</v>
+        <v>7100</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2995,11 +2995,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="44">
+        <v>52</v>
+      </c>
       <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2600</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3012,11 +3014,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="44">
+        <v>40</v>
+      </c>
       <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3029,13 +3033,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44">
-        <v>190</v>
-      </c>
+      <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3052,7 +3054,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>140000</v>
+        <v>128000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3326,12 +3328,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="44">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>64000</v>
+        <v>42000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3345,12 +3347,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="44">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>66000</v>
+        <v>75500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3364,12 +3366,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="44">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>8100</v>
+        <v>7100</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3382,11 +3384,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
+      <c r="E36" s="44">
+        <v>52</v>
+      </c>
       <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2600</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3399,11 +3403,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
+      <c r="E37" s="44">
+        <v>40</v>
+      </c>
       <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3416,13 +3422,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44">
-        <v>190</v>
-      </c>
+      <c r="E38" s="44"/>
       <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1900</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3439,7 +3443,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>140000</v>
+        <v>128000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
18.09.19 Today Salses Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -101,10 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Date: 17.09.19</t>
+    <t>Date: 18.09.19</t>
   </si>
 </sst>
 </file>
@@ -399,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -476,12 +473,48 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -491,90 +524,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -582,35 +588,42 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,16 +826,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1609725</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -831,8 +844,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="47625" y="4829175"/>
-          <a:ext cx="1190625" cy="9525"/>
+          <a:off x="1504950" y="5343525"/>
+          <a:ext cx="1343025" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -901,14 +914,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1562100</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>11113</xdr:rowOff>
     </xdr:to>
@@ -919,7 +932,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="12382500"/>
+          <a:off x="1571625" y="12744450"/>
           <a:ext cx="1228725" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2057,7 +2070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2079,60 +2092,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2141,10 +2154,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2159,10 +2172,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="37">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2178,10 +2191,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="37">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2197,10 +2210,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="37">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2216,10 +2229,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="37">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2235,8 +2248,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2252,8 +2265,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2266,10 +2279,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2316,58 +2329,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2377,11 +2390,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2456,60 +2469,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2518,10 +2531,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2536,10 +2549,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="37">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2555,10 +2568,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="37">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2574,10 +2587,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="37">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2593,10 +2606,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="37">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2612,8 +2625,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2629,8 +2642,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2643,10 +2656,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2693,58 +2706,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2754,11 +2767,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2786,6 +2799,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2798,32 +2837,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2835,8 +2848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="K47" sqref="A1:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2854,63 +2867,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="A4" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2920,10 +2933,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="56"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2938,13 +2951,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>42</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="57">
+        <v>6</v>
+      </c>
+      <c r="F6" s="57"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>42000</v>
+        <v>6000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2957,13 +2970,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>151</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="57">
+        <v>249</v>
+      </c>
+      <c r="F7" s="57"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>75500</v>
+        <v>124500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2976,13 +2989,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>71</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="57">
+        <v>314</v>
+      </c>
+      <c r="F8" s="57"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>7100</v>
+        <v>31400</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2995,13 +3008,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>52</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="57">
+        <v>22</v>
+      </c>
+      <c r="F9" s="57"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>2600</v>
+        <v>1100</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3014,13 +3027,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>40</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="57">
+        <v>100</v>
+      </c>
+      <c r="F10" s="57"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3033,11 +3046,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="57">
+        <v>200</v>
+      </c>
+      <c r="F11" s="57"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3047,14 +3062,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="58"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>128000</v>
+        <v>167000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3085,118 +3100,118 @@
       <c r="J14" s="26"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="78"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="49" t="s">
         <v>7</v>
-      </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
-        <v>8</v>
       </c>
       <c r="I16" s="49"/>
       <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
       <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31" t="s">
         <v>12</v>
       </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="50"/>
       <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="26"/>
@@ -3247,60 +3262,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="A31" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3309,10 +3324,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3327,13 +3342,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>42</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="57">
+        <v>6</v>
+      </c>
+      <c r="F33" s="57"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>42000</v>
+        <v>6000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3346,13 +3361,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>151</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="57">
+        <v>249</v>
+      </c>
+      <c r="F34" s="57"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>75500</v>
+        <v>124500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3365,13 +3380,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>71</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="57">
+        <v>314</v>
+      </c>
+      <c r="F35" s="57"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>7100</v>
+        <v>31400</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3384,13 +3399,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>52</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="57">
+        <v>22</v>
+      </c>
+      <c r="F36" s="57"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>2600</v>
+        <v>1100</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3403,13 +3418,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>40</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="57">
+        <v>100</v>
+      </c>
+      <c r="F37" s="57"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3422,11 +3437,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="57">
+        <v>200</v>
+      </c>
+      <c r="F38" s="57"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3436,14 +3453,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="52"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>128000</v>
+        <v>167000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3474,8 +3491,8 @@
       <c r="J41" s="26"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
@@ -3486,56 +3503,56 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="49"/>
+      <c r="A43" s="78"/>
+      <c r="B43" s="78"/>
       <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
+      <c r="D43" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
       <c r="H43" s="49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I43" s="49"/>
       <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="79"/>
+      <c r="B44" s="79"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="79"/>
+      <c r="B45" s="79"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="78"/>
+      <c r="B46" s="78"/>
       <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
+      <c r="D46" s="31" t="s">
+        <v>12</v>
+      </c>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
-        <v>25</v>
-      </c>
+      <c r="H46" s="50"/>
       <c r="I46" s="50"/>
       <c r="J46" s="50"/>
     </row>
@@ -3547,9 +3564,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3576,12 +3593,30 @@
       <c r="J49" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="34">
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="A46:B46"/>
     <mergeCell ref="H43:J43"/>
     <mergeCell ref="H44:J45"/>
     <mergeCell ref="H46:J46"/>
@@ -3593,28 +3628,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3645,63 +3658,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3711,10 +3724,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3729,10 +3742,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="37">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3748,10 +3761,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="37">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3767,10 +3780,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="37">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3786,10 +3799,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="37">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3805,10 +3818,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="37">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3824,8 +3837,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3838,10 +3851,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3888,76 +3901,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4032,60 +4045,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4094,10 +4107,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="63"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4112,10 +4125,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="62">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4131,10 +4144,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="62">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4150,10 +4163,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="62">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="62"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4169,10 +4182,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="62">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="62"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4188,10 +4201,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="62">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4207,8 +4220,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4221,10 +4234,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4271,76 +4284,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="60"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4368,6 +4381,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4384,30 +4421,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4439,63 +4452,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4505,10 +4518,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4523,10 +4536,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="37">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4542,10 +4555,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="37">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4561,10 +4574,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="37">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4580,8 +4593,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4597,8 +4610,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4614,8 +4627,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4628,10 +4641,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4678,72 +4691,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4818,60 +4831,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4880,10 +4893,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4898,10 +4911,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="37">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4917,10 +4930,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="37">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4936,10 +4949,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="37">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4955,8 +4968,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4972,8 +4985,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4989,8 +5002,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5003,10 +5016,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5053,72 +5066,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="60"/>
+      <c r="B46" s="60"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5146,16 +5159,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5168,24 +5189,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5210,64 +5223,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5278,8 +5291,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5290,8 +5303,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5302,8 +5315,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5314,8 +5327,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5326,8 +5339,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5338,8 +5351,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5349,8 +5362,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5394,52 +5407,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5449,9 +5462,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5538,60 +5551,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5602,10 +5615,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="63"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5620,10 +5633,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="37">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5639,10 +5652,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="37">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5658,10 +5671,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="37">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5677,8 +5690,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5694,8 +5707,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5711,10 +5724,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="62">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5727,10 +5740,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="63" t="s">
+      <c r="D39" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="64"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5777,58 +5790,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5838,12 +5851,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5856,32 +5895,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5907,177 +5920,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="76">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="75">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="76">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="75">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="75"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="76">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="75">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="76">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="75">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="75"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="75">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="75"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6088,10 +6101,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="63"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6106,8 +6119,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6123,10 +6136,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="37">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6142,8 +6155,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6159,10 +6172,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="37">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="37"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6178,8 +6191,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6195,10 +6208,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="62">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6211,10 +6224,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="64"/>
+      <c r="E32" s="67"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6261,58 +6274,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6322,12 +6335,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6344,23 +6374,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
19.09.19 Today SALES DE
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 18.09.19</t>
+    <t>Date: 19.09.19</t>
   </si>
 </sst>
 </file>
@@ -482,82 +482,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -572,15 +582,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -588,6 +595,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -609,21 +622,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2070,7 +2070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2092,60 +2092,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2154,10 +2154,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2172,10 +2172,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2191,10 +2191,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2210,10 +2210,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2229,10 +2229,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2248,8 +2248,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2265,8 +2265,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2279,10 +2279,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2329,58 +2329,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2390,11 +2390,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2469,60 +2469,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2531,10 +2531,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2549,10 +2549,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="37">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2568,10 +2568,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="37"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2587,10 +2587,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="37">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="37"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2606,10 +2606,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="37">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="37"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2625,8 +2625,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2642,8 +2642,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2656,10 +2656,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="45"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2706,58 +2706,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="46"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="46" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="39" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2767,11 +2767,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2799,14 +2799,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2819,24 +2829,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2848,8 +2848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="K47" sqref="A1:K47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2867,63 +2867,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2933,10 +2933,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="56"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2951,13 +2951,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="57">
-        <v>6</v>
-      </c>
-      <c r="F6" s="57"/>
+      <c r="E6" s="51">
+        <v>74</v>
+      </c>
+      <c r="F6" s="51"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>6000</v>
+        <v>74000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2970,13 +2970,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="57">
-        <v>249</v>
-      </c>
-      <c r="F7" s="57"/>
+      <c r="E7" s="51">
+        <v>125</v>
+      </c>
+      <c r="F7" s="51"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>124500</v>
+        <v>62500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2989,13 +2989,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="57">
-        <v>314</v>
-      </c>
-      <c r="F8" s="57"/>
+      <c r="E8" s="51">
+        <v>294</v>
+      </c>
+      <c r="F8" s="51"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>31400</v>
+        <v>29400</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3008,13 +3008,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="57">
-        <v>22</v>
-      </c>
-      <c r="F9" s="57"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3027,13 +3025,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="57">
-        <v>100</v>
-      </c>
-      <c r="F10" s="57"/>
+      <c r="E10" s="51">
+        <v>205</v>
+      </c>
+      <c r="F10" s="51"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>4100</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3046,10 +3044,10 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="51">
         <v>200</v>
       </c>
-      <c r="F11" s="57"/>
+      <c r="F11" s="51"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>2000</v>
@@ -3062,14 +3060,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="58"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>167000</v>
+        <v>172000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3112,48 +3110,48 @@
       <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="78"/>
-      <c r="B16" s="78"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="78"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="78"/>
-      <c r="B17" s="78"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="49"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="78"/>
-      <c r="B18" s="78"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="49"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="78"/>
-      <c r="B19" s="78"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="30"/>
       <c r="D19" s="31" t="s">
         <v>12</v>
@@ -3161,9 +3159,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="32"/>
@@ -3173,9 +3171,9 @@
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="32"/>
@@ -3262,60 +3260,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3324,10 +3322,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3342,13 +3340,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="57">
-        <v>6</v>
-      </c>
-      <c r="F33" s="57"/>
+      <c r="E33" s="51">
+        <v>74</v>
+      </c>
+      <c r="F33" s="51"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>6000</v>
+        <v>74000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3361,13 +3359,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="57">
-        <v>249</v>
-      </c>
-      <c r="F34" s="57"/>
+      <c r="E34" s="51">
+        <v>125</v>
+      </c>
+      <c r="F34" s="51"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>124500</v>
+        <v>62500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3380,13 +3378,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="57">
-        <v>314</v>
-      </c>
-      <c r="F35" s="57"/>
+      <c r="E35" s="51">
+        <v>294</v>
+      </c>
+      <c r="F35" s="51"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>31400</v>
+        <v>29400</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3399,13 +3397,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="57">
-        <v>22</v>
-      </c>
-      <c r="F36" s="57"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3418,13 +3414,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="57">
-        <v>100</v>
-      </c>
-      <c r="F37" s="57"/>
+      <c r="E37" s="51">
+        <v>205</v>
+      </c>
+      <c r="F37" s="51"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2000</v>
+        <v>4100</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3437,10 +3433,10 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="57">
+      <c r="E38" s="51">
         <v>200</v>
       </c>
-      <c r="F38" s="57"/>
+      <c r="F38" s="51"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>2000</v>
@@ -3453,14 +3449,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="51" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="52"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>167000</v>
+        <v>172000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3503,8 +3499,8 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="78"/>
-      <c r="B43" s="78"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28" t="s">
         <v>8</v>
@@ -3512,39 +3508,39 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="79"/>
-      <c r="B44" s="79"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="48"/>
+      <c r="D44" s="49"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="79"/>
-      <c r="B45" s="79"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="48"/>
+      <c r="D45" s="49"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="78"/>
-      <c r="B46" s="78"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="28"/>
       <c r="D46" s="31" t="s">
         <v>12</v>
@@ -3552,9 +3548,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3564,9 +3560,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3594,33 +3590,11 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
     <mergeCell ref="H44:J45"/>
     <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D39:E39"/>
     <mergeCell ref="A28:J28"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A30:J30"/>
@@ -3628,6 +3602,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D39:E39"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3658,63 +3654,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3724,10 +3720,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3742,10 +3738,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3761,10 +3757,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3780,10 +3776,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3799,10 +3795,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="37"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3818,10 +3814,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3837,8 +3833,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3851,10 +3847,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3901,76 +3897,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="59"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4045,60 +4041,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4107,10 +4103,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="63" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="63"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4125,10 +4121,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="62">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4144,10 +4140,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="62"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4163,10 +4159,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="62"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4182,10 +4178,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="62"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4201,10 +4197,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="62">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="62"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4220,8 +4216,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4234,10 +4230,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4284,76 +4280,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="46"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="46" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="39"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="39" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="60"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4381,30 +4377,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4421,6 +4393,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4452,63 +4448,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4518,10 +4514,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4536,10 +4532,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4555,10 +4551,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4574,10 +4570,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4593,8 +4589,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4610,8 +4606,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4627,8 +4623,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4641,10 +4637,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4691,72 +4687,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="65"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4831,60 +4827,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4893,10 +4889,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4911,10 +4907,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="37">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4930,10 +4926,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="37"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4949,10 +4945,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="37">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="37"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4968,8 +4964,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4985,8 +4981,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5002,8 +4998,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5016,10 +5012,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5066,72 +5062,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="46"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="46" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="39" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="60"/>
-      <c r="B46" s="60"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5159,6 +5155,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5171,34 +5195,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5223,64 +5219,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5291,8 +5287,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5303,8 +5299,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5315,8 +5311,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5327,8 +5323,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5339,8 +5335,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5351,8 +5347,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5362,8 +5358,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5407,52 +5403,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5462,9 +5458,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5551,60 +5547,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5615,10 +5611,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="63"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5633,10 +5629,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="37"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5652,10 +5648,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="37">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="37"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5671,10 +5667,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="37">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="37"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5690,8 +5686,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5707,8 +5703,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5724,10 +5720,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="62">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="62"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5740,10 +5736,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="67"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5790,58 +5786,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="39" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5851,20 +5847,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5877,24 +5883,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5920,177 +5916,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="76">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="75">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="76"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="75"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="76">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="75">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="76"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="75"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="76">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="75">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="76"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="75"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="76">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="75">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="76"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="75">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="75"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6101,10 +6097,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="63" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="63"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6119,8 +6115,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6136,10 +6132,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="37"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6155,8 +6151,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6172,10 +6168,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="37"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6191,8 +6187,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6208,10 +6204,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="62">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6224,10 +6220,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="66" t="s">
+      <c r="D32" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="67"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6274,58 +6270,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="46"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="46" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="39" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6335,29 +6331,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6374,6 +6353,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
21.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 19.09.19</t>
+    <t>Date: 21.09.19</t>
   </si>
 </sst>
 </file>
@@ -488,12 +488,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -503,91 +530,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -595,12 +595,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,6 +616,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2070,7 +2070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2092,60 +2092,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2154,10 +2154,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2172,10 +2172,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2191,10 +2191,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2210,10 +2210,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2229,10 +2229,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2248,8 +2248,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2265,8 +2265,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2279,10 +2279,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2329,58 +2329,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2390,11 +2390,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2469,60 +2469,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2531,10 +2531,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2549,10 +2549,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2568,10 +2568,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2587,10 +2587,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2606,10 +2606,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2625,8 +2625,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2642,8 +2642,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2656,10 +2656,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2706,58 +2706,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2767,11 +2767,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2799,6 +2799,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2811,32 +2837,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2867,63 +2867,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2933,10 +2933,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="55"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2951,13 +2951,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="51">
-        <v>74</v>
-      </c>
-      <c r="F6" s="51"/>
+      <c r="E6" s="58">
+        <v>46</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>74000</v>
+        <v>46000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2970,13 +2970,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="51">
-        <v>125</v>
-      </c>
-      <c r="F7" s="51"/>
+      <c r="E7" s="58">
+        <v>153</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>62500</v>
+        <v>76500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2989,13 +2989,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="51">
-        <v>294</v>
-      </c>
-      <c r="F8" s="51"/>
+      <c r="E8" s="58">
+        <v>95</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>29400</v>
+        <v>9500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3008,11 +3008,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="E9" s="58">
+        <v>20</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3025,13 +3027,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="51">
-        <v>205</v>
-      </c>
-      <c r="F10" s="51"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>4100</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3044,13 +3044,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="51">
-        <v>200</v>
-      </c>
-      <c r="F11" s="51"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3060,14 +3058,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="57"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>172000</v>
+        <v>133000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3119,35 +3117,35 @@
       <c r="E16" s="33"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="33"/>
       <c r="B17" s="33"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="50"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="33"/>
       <c r="B18" s="33"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="33"/>
@@ -3159,9 +3157,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="32"/>
@@ -3171,9 +3169,9 @@
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="32"/>
@@ -3260,60 +3258,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3322,10 +3320,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="55"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3340,13 +3338,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="51">
-        <v>74</v>
-      </c>
-      <c r="F33" s="51"/>
+      <c r="E33" s="58">
+        <v>46</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>74000</v>
+        <v>46000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3359,13 +3357,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="51">
-        <v>125</v>
-      </c>
-      <c r="F34" s="51"/>
+      <c r="E34" s="58">
+        <v>153</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>62500</v>
+        <v>76500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3378,13 +3376,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="51">
-        <v>294</v>
-      </c>
-      <c r="F35" s="51"/>
+      <c r="E35" s="58">
+        <v>95</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>29400</v>
+        <v>9500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3397,11 +3395,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
+      <c r="E36" s="58">
+        <v>20</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3414,13 +3414,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="51">
-        <v>205</v>
-      </c>
-      <c r="F37" s="51"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>4100</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3433,13 +3431,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="51">
-        <v>200</v>
-      </c>
-      <c r="F38" s="51"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3456,7 +3452,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>172000</v>
+        <v>133000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3508,35 +3504,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="50" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="34"/>
       <c r="B44" s="34"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="49"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-      <c r="J44" s="49"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="34"/>
       <c r="B45" s="34"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="49"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="49"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="33"/>
@@ -3548,9 +3544,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3560,9 +3556,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3590,6 +3586,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3602,27 +3618,7 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="D39:E39"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3654,63 +3650,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3720,10 +3716,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3738,10 +3734,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3757,10 +3753,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3776,10 +3772,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3795,10 +3791,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3814,10 +3810,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3833,8 +3829,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3847,10 +3843,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3897,76 +3893,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4041,60 +4037,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4103,10 +4099,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4121,10 +4117,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4140,10 +4136,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4159,10 +4155,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4178,10 +4174,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4197,10 +4193,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4216,8 +4212,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4230,10 +4226,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4280,76 +4276,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4377,6 +4373,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4393,30 +4413,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4448,63 +4444,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4514,10 +4510,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4532,10 +4528,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4551,10 +4547,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4570,10 +4566,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4589,8 +4585,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4606,8 +4602,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4623,8 +4619,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4637,10 +4633,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4687,72 +4683,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4827,60 +4823,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4889,10 +4885,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4907,10 +4903,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4926,10 +4922,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4945,10 +4941,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4964,8 +4960,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4981,8 +4977,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4998,8 +4994,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5012,10 +5008,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5062,72 +5058,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5155,16 +5151,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5177,24 +5181,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5219,64 +5215,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5287,8 +5283,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5299,8 +5295,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5311,8 +5307,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5323,8 +5319,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5335,8 +5331,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5347,8 +5343,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5358,8 +5354,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5403,52 +5399,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5458,9 +5454,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5547,60 +5543,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5611,10 +5607,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5629,10 +5625,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5648,10 +5644,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5667,10 +5663,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5686,8 +5682,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5703,8 +5699,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5720,10 +5716,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5786,58 +5782,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5847,12 +5843,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5865,32 +5887,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5916,177 +5912,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6097,10 +6093,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6115,8 +6111,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6132,10 +6128,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6151,8 +6147,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6168,10 +6164,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6187,8 +6183,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6204,10 +6200,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6270,58 +6266,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6331,12 +6327,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6353,23 +6366,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
22.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Date: 21.09.19</t>
+  </si>
+  <si>
+    <t>Date: 22.09.19</t>
   </si>
 </sst>
 </file>
@@ -558,13 +561,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2848,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2913,7 +2916,7 @@
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
       <c r="A4" s="56" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
@@ -2952,12 +2955,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="58">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>46000</v>
+        <v>36000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2971,12 +2974,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="58">
-        <v>153</v>
+        <v>67</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>76500</v>
+        <v>33500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2990,12 +2993,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="58">
-        <v>95</v>
+        <v>387</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>9500</v>
+        <v>38700</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3009,12 +3012,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="58">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3027,11 +3030,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58"/>
+      <c r="E10" s="58">
+        <v>200</v>
+      </c>
       <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3044,11 +3049,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58"/>
+      <c r="E11" s="58">
+        <v>10</v>
+      </c>
       <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3058,14 +3065,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="59"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>133000</v>
+        <v>114000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3339,12 +3346,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="58">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>46000</v>
+        <v>36000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3358,12 +3365,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="58">
-        <v>153</v>
+        <v>67</v>
       </c>
       <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>76500</v>
+        <v>33500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3377,12 +3384,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="58">
-        <v>95</v>
+        <v>387</v>
       </c>
       <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>9500</v>
+        <v>38700</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3396,12 +3403,12 @@
         <v>50</v>
       </c>
       <c r="E36" s="58">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3414,11 +3421,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58"/>
+      <c r="E37" s="58">
+        <v>200</v>
+      </c>
       <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3431,11 +3440,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="58">
+        <v>10</v>
+      </c>
       <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3445,14 +3456,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>133000</v>
+        <v>114000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
23.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -101,10 +101,10 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 21.09.19</t>
+    <t>Date: 23.09.19</t>
   </si>
   <si>
-    <t>Date: 22.09.19</t>
+    <t>Rahinul Islam</t>
   </si>
 </sst>
 </file>
@@ -479,95 +479,98 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -582,15 +585,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,6 +598,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,12 +625,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,60 +2095,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2157,10 +2157,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2194,10 +2194,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2213,10 +2213,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2232,10 +2232,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2251,8 +2251,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2268,8 +2268,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2282,10 +2282,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2332,58 +2332,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2393,11 +2393,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2472,60 +2472,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2534,10 +2534,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2552,10 +2552,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2571,10 +2571,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2590,10 +2590,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2609,10 +2609,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2628,8 +2628,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2645,8 +2645,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2659,10 +2659,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2709,58 +2709,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2770,11 +2770,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2802,14 +2802,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2822,24 +2832,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2870,63 +2870,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="A4" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2936,10 +2936,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2954,13 +2954,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>36</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>25</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>36000</v>
+        <v>25000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>67</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>208</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>33500</v>
+        <v>104000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>387</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>394</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>38700</v>
+        <v>39400</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>34</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>14</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3030,13 +3030,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>200</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>40</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>800</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3049,10 +3049,10 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="53">
         <v>10</v>
       </c>
-      <c r="F11" s="58"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3065,14 +3065,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>114000</v>
+        <v>170000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3103,118 +3103,118 @@
       <c r="J14" s="26"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="33"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="30"/>
-      <c r="D19" s="31" t="s">
-        <v>12</v>
+      <c r="D19" s="34" t="s">
+        <v>26</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="26"/>
@@ -3265,60 +3265,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3327,10 +3327,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3345,13 +3345,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>36</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>25</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>36000</v>
+        <v>25000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3364,13 +3364,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>67</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>208</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>33500</v>
+        <v>104000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3383,13 +3383,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>387</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>394</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>38700</v>
+        <v>39400</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3402,13 +3402,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>34</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>14</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3421,13 +3421,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>200</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>40</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>4000</v>
+        <v>800</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3440,10 +3440,10 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58">
+      <c r="E38" s="53">
         <v>10</v>
       </c>
-      <c r="F38" s="58"/>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3456,14 +3456,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>114000</v>
+        <v>170000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3494,8 +3494,8 @@
       <c r="J41" s="26"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
@@ -3506,8 +3506,8 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28" t="s">
         <v>8</v>
@@ -3515,49 +3515,49 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="28"/>
-      <c r="D46" s="31" t="s">
-        <v>12</v>
+      <c r="D46" s="34" t="s">
+        <v>26</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3567,9 +3567,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3597,26 +3597,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3631,6 +3611,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3661,63 +3661,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3727,10 +3727,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3745,10 +3745,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3764,10 +3764,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3783,10 +3783,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3802,10 +3802,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3821,10 +3821,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3840,8 +3840,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3854,10 +3854,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3904,76 +3904,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4048,60 +4048,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4110,10 +4110,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4128,10 +4128,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4147,10 +4147,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4166,10 +4166,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4185,10 +4185,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4204,10 +4204,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4223,8 +4223,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4237,10 +4237,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4287,76 +4287,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4384,30 +4384,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4424,6 +4400,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4455,63 +4455,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4521,10 +4521,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4539,10 +4539,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4558,10 +4558,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4577,10 +4577,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4596,8 +4596,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4613,8 +4613,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4630,8 +4630,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4644,10 +4644,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4694,72 +4694,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4834,60 +4834,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4896,10 +4896,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4914,10 +4914,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4933,10 +4933,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4952,10 +4952,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4971,8 +4971,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4988,8 +4988,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5005,8 +5005,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5019,10 +5019,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5069,72 +5069,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5162,6 +5162,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5174,34 +5202,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5226,64 +5226,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5294,8 +5294,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5306,8 +5306,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5318,8 +5318,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5330,8 +5330,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5342,8 +5342,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5354,8 +5354,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5365,8 +5365,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5410,52 +5410,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5465,9 +5465,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5554,60 +5554,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5618,10 +5618,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5636,10 +5636,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5655,10 +5655,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5674,10 +5674,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5693,8 +5693,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5710,8 +5710,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5727,10 +5727,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5793,58 +5793,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5854,20 +5854,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5880,24 +5890,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5923,177 +5923,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6104,10 +6104,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6122,8 +6122,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6139,10 +6139,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6158,8 +6158,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6175,10 +6175,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6194,8 +6194,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6211,10 +6211,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6277,58 +6277,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6338,29 +6338,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6377,6 +6360,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
25.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t>Rahinul Islam</t>
   </si>
   <si>
-    <t>Date: 24.09.19</t>
+    <t>Date: 25.09.19</t>
   </si>
 </sst>
 </file>
@@ -491,83 +491,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -582,15 +585,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,6 +598,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,12 +625,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,60 +2095,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2157,10 +2157,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2194,10 +2194,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2213,10 +2213,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2232,10 +2232,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2251,8 +2251,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2268,8 +2268,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2282,10 +2282,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2332,58 +2332,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2393,11 +2393,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2472,60 +2472,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2534,10 +2534,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2552,10 +2552,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2571,10 +2571,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2590,10 +2590,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2609,10 +2609,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2628,8 +2628,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2645,8 +2645,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2659,10 +2659,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2709,58 +2709,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2770,11 +2770,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2802,14 +2802,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2822,24 +2832,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2870,63 +2870,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2936,10 +2936,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2954,13 +2954,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>102</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>121</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>102000</v>
+        <v>121000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>134</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>253</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>67000</v>
+        <v>126500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>200</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>419</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>41900</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>18</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>14</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3030,13 +3030,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>55</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>35</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3049,11 +3049,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53">
+        <v>20</v>
+      </c>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3063,14 +3065,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>191000</v>
+        <v>291000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3122,35 +3124,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3162,9 +3164,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3174,9 +3176,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3263,60 +3265,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3325,10 +3327,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3343,13 +3345,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>102</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>121</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>102000</v>
+        <v>121000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3362,13 +3364,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>134</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>253</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>67000</v>
+        <v>126500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3381,13 +3383,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>200</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>419</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>41900</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3400,13 +3402,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>18</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>14</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3419,13 +3421,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>55</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>35</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3438,11 +3440,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53">
+        <v>20</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3452,14 +3456,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>191000</v>
+        <v>291000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3511,35 +3515,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3551,9 +3555,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3563,9 +3567,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3593,26 +3597,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3627,6 +3611,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3657,63 +3661,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3723,10 +3727,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3741,10 +3745,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3760,10 +3764,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3779,10 +3783,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3798,10 +3802,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,10 +3821,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3836,8 +3840,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3850,10 +3854,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3900,76 +3904,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4044,60 +4048,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4106,10 +4110,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4124,10 +4128,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4143,10 +4147,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4162,10 +4166,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4181,10 +4185,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,10 +4204,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4219,8 +4223,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4233,10 +4237,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4283,76 +4287,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4380,30 +4384,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4420,6 +4400,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4451,63 +4455,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4517,10 +4521,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4535,10 +4539,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4554,10 +4558,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4573,10 +4577,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4592,8 +4596,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4609,8 +4613,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4626,8 +4630,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4640,10 +4644,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4690,72 +4694,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4830,60 +4834,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4892,10 +4896,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4910,10 +4914,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4929,10 +4933,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4948,10 +4952,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4967,8 +4971,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4984,8 +4988,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5001,8 +5005,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5015,10 +5019,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5065,72 +5069,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5158,6 +5162,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5170,34 +5202,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5222,64 +5226,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5290,8 +5294,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5302,8 +5306,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5314,8 +5318,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5326,8 +5330,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5338,8 +5342,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5350,8 +5354,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5361,8 +5365,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5406,52 +5410,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5461,9 +5465,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5550,60 +5554,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5614,10 +5618,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5632,10 +5636,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5651,10 +5655,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5670,10 +5674,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5689,8 +5693,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5706,8 +5710,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5723,10 +5727,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5789,58 +5793,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5850,20 +5854,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5876,24 +5890,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5919,177 +5923,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6100,10 +6104,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6118,8 +6122,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6135,10 +6139,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6154,8 +6158,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6171,10 +6175,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6190,8 +6194,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6207,10 +6211,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6273,58 +6277,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6334,29 +6338,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6373,6 +6360,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
26.09.19 Today Sales Detauls
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t>Rahinul Islam</t>
   </si>
   <si>
-    <t>Date: 25.09.19</t>
+    <t>Date: 26.09.19</t>
   </si>
 </sst>
 </file>
@@ -491,12 +491,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -506,32 +533,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -548,49 +561,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,12 +598,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,6 +619,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,60 +2095,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2157,10 +2157,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2194,10 +2194,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2213,10 +2213,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2232,10 +2232,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2251,8 +2251,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2268,8 +2268,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2282,10 +2282,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2332,58 +2332,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2393,11 +2393,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2472,60 +2472,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2534,10 +2534,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2552,10 +2552,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2571,10 +2571,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2590,10 +2590,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2609,10 +2609,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2628,8 +2628,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2645,8 +2645,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2659,10 +2659,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2709,58 +2709,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2770,11 +2770,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2802,6 +2802,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2814,32 +2840,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2852,7 +2852,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+      <selection activeCell="K47" sqref="A1:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2870,63 +2870,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2936,10 +2936,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2954,13 +2954,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>121</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>43</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>121000</v>
+        <v>43000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>253</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>225</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>126500</v>
+        <v>112500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>419</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>125</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>41900</v>
+        <v>12500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>14</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>10</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3030,13 +3030,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>35</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3049,13 +3047,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>20</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58">
+        <v>150</v>
+      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3065,14 +3063,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>291000</v>
+        <v>170000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3124,35 +3122,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3164,9 +3162,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3176,9 +3174,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3265,60 +3263,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3327,10 +3325,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3345,13 +3343,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>121</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>43</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>121000</v>
+        <v>43000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3364,13 +3362,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>253</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>225</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>126500</v>
+        <v>112500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3383,13 +3381,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>419</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>125</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>41900</v>
+        <v>12500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3402,13 +3400,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>14</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>10</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3421,13 +3419,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>35</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3440,13 +3436,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>20</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58">
+        <v>150</v>
+      </c>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3456,14 +3452,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>291000</v>
+        <v>170000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3515,35 +3511,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3555,9 +3551,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3567,9 +3563,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3597,6 +3593,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3611,26 +3627,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3661,63 +3657,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3727,10 +3723,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3745,10 +3741,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3764,10 +3760,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3783,10 +3779,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3802,10 +3798,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3821,10 +3817,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3840,8 +3836,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3854,10 +3850,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3904,76 +3900,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4048,60 +4044,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4110,10 +4106,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4128,10 +4124,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4147,10 +4143,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4166,10 +4162,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4185,10 +4181,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4204,10 +4200,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4223,8 +4219,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4237,10 +4233,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4287,76 +4283,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4384,6 +4380,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4400,30 +4420,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4455,63 +4451,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4521,10 +4517,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4539,10 +4535,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4558,10 +4554,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4577,10 +4573,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4596,8 +4592,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4613,8 +4609,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4630,8 +4626,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4644,10 +4640,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4694,72 +4690,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4834,60 +4830,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4896,10 +4892,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4914,10 +4910,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4933,10 +4929,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4952,10 +4948,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4971,8 +4967,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4988,8 +4984,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5005,8 +5001,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5019,10 +5015,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5069,72 +5065,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5162,16 +5158,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5184,24 +5188,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5226,64 +5222,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5294,8 +5290,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5306,8 +5302,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5318,8 +5314,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5330,8 +5326,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5342,8 +5338,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5354,8 +5350,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5365,8 +5361,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5410,52 +5406,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5465,9 +5461,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5554,60 +5550,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5618,10 +5614,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5636,10 +5632,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5655,10 +5651,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5674,10 +5670,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5693,8 +5689,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5710,8 +5706,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5727,10 +5723,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5793,58 +5789,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5854,12 +5850,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5872,32 +5894,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5923,177 +5919,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6104,10 +6100,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6122,8 +6118,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6139,10 +6135,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6158,8 +6154,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6175,10 +6171,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6194,8 +6190,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6211,10 +6207,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6277,58 +6273,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6338,12 +6334,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6360,23 +6373,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
28.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t>Rahinul Islam</t>
   </si>
   <si>
-    <t>Date: 26.09.19</t>
+    <t>Date: 28.09.19</t>
   </si>
 </sst>
 </file>
@@ -491,83 +491,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -582,15 +585,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,6 +598,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,12 +625,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,60 +2095,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2157,10 +2157,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2194,10 +2194,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2213,10 +2213,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2232,10 +2232,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2251,8 +2251,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2268,8 +2268,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2282,10 +2282,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2332,58 +2332,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2393,11 +2393,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2472,60 +2472,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2534,10 +2534,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2552,10 +2552,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2571,10 +2571,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2590,10 +2590,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2609,10 +2609,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2628,8 +2628,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2645,8 +2645,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2659,10 +2659,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2709,58 +2709,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2770,11 +2770,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2802,14 +2802,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2822,24 +2832,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="A1:K47"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2870,63 +2870,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2936,10 +2936,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2954,13 +2954,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>43</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>46</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>43000</v>
+        <v>46000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>225</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>193</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>112500</v>
+        <v>96500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>125</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>164</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>12500</v>
+        <v>16400</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>10</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>100</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3030,11 +3030,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>115</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3047,13 +3049,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58">
-        <v>150</v>
-      </c>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53">
+        <v>80</v>
+      </c>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>800</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3063,14 +3065,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>170000</v>
+        <v>167000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3122,35 +3124,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3162,9 +3164,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3174,9 +3176,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3263,60 +3265,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3325,10 +3327,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3343,13 +3345,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>43</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>46</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>43000</v>
+        <v>46000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3362,13 +3364,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>225</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>193</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>112500</v>
+        <v>96500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3381,13 +3383,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>125</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>164</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>12500</v>
+        <v>16400</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3400,13 +3402,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>10</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>100</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3419,11 +3421,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>115</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3436,13 +3440,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58">
-        <v>150</v>
-      </c>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53">
+        <v>80</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>800</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3452,14 +3456,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>170000</v>
+        <v>167000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3511,35 +3515,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3551,9 +3555,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3563,9 +3567,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3593,26 +3597,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3627,6 +3611,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3657,63 +3661,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3723,10 +3727,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3741,10 +3745,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3760,10 +3764,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3779,10 +3783,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3798,10 +3802,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,10 +3821,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3836,8 +3840,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3850,10 +3854,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3900,76 +3904,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4044,60 +4048,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4106,10 +4110,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4124,10 +4128,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4143,10 +4147,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4162,10 +4166,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4181,10 +4185,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,10 +4204,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4219,8 +4223,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4233,10 +4237,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4283,76 +4287,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4380,30 +4384,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4420,6 +4400,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4451,63 +4455,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4517,10 +4521,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4535,10 +4539,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4554,10 +4558,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4573,10 +4577,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4592,8 +4596,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4609,8 +4613,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4626,8 +4630,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4640,10 +4644,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4690,72 +4694,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4830,60 +4834,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4892,10 +4896,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4910,10 +4914,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4929,10 +4933,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4948,10 +4952,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4967,8 +4971,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4984,8 +4988,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5001,8 +5005,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5015,10 +5019,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5065,72 +5069,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5158,6 +5162,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5170,34 +5202,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5222,64 +5226,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5290,8 +5294,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5302,8 +5306,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5314,8 +5318,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5326,8 +5330,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5338,8 +5342,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5350,8 +5354,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5361,8 +5365,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5406,52 +5410,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5461,9 +5465,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5550,60 +5554,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5614,10 +5618,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5632,10 +5636,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5651,10 +5655,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5670,10 +5674,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5689,8 +5693,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5706,8 +5710,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5723,10 +5727,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5789,58 +5793,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5850,20 +5854,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5876,24 +5890,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5919,177 +5923,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6100,10 +6104,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6118,8 +6122,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6135,10 +6139,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6154,8 +6158,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6171,10 +6175,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6190,8 +6194,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6207,10 +6211,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6273,58 +6277,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6334,29 +6338,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6373,6 +6360,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
29.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t>Rahinul Islam</t>
   </si>
   <si>
-    <t>Date: 28.09.19</t>
+    <t>Date: 29.09.19</t>
   </si>
 </sst>
 </file>
@@ -491,12 +491,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -506,32 +533,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -548,49 +561,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,12 +598,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,6 +619,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,60 +2095,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2157,10 +2157,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2194,10 +2194,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2213,10 +2213,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2232,10 +2232,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2251,8 +2251,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2268,8 +2268,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2282,10 +2282,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2332,58 +2332,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2393,11 +2393,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2472,60 +2472,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2534,10 +2534,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2552,10 +2552,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2571,10 +2571,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2590,10 +2590,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2609,10 +2609,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2628,8 +2628,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2645,8 +2645,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2659,10 +2659,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2709,58 +2709,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2770,11 +2770,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2802,6 +2802,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2814,32 +2840,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2870,63 +2870,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2936,10 +2936,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2954,13 +2954,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>46</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>103</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>46000</v>
+        <v>103000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>193</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>228</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>96500</v>
+        <v>114000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>164</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>262</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>16400</v>
+        <v>26200</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>100</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>27</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>1350</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3030,13 +3030,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>115</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>10</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2300</v>
+        <v>200</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3049,13 +3049,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>80</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58">
+        <v>125</v>
+      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>1250</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3065,14 +3065,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>167000</v>
+        <v>246000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3124,35 +3124,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3164,9 +3164,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3176,9 +3176,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3265,60 +3265,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3327,10 +3327,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3345,13 +3345,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>46</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>103</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>46000</v>
+        <v>103000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3364,13 +3364,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>193</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>228</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>96500</v>
+        <v>114000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3383,13 +3383,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>164</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>262</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>16400</v>
+        <v>26200</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3402,13 +3402,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>100</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>27</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>1350</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3421,13 +3421,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>115</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>10</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2300</v>
+        <v>200</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3440,13 +3440,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>80</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58">
+        <v>125</v>
+      </c>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>1250</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3456,14 +3456,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>167000</v>
+        <v>246000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3515,35 +3515,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3555,9 +3555,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3567,9 +3567,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3597,6 +3597,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3611,26 +3631,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3661,63 +3661,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3727,10 +3727,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3745,10 +3745,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3764,10 +3764,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3783,10 +3783,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3802,10 +3802,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3821,10 +3821,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3840,8 +3840,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3854,10 +3854,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3904,76 +3904,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4048,60 +4048,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4110,10 +4110,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4128,10 +4128,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4147,10 +4147,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4166,10 +4166,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4185,10 +4185,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4204,10 +4204,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4223,8 +4223,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4237,10 +4237,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4287,76 +4287,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4384,6 +4384,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4400,30 +4424,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4455,63 +4455,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4521,10 +4521,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4539,10 +4539,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4558,10 +4558,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4577,10 +4577,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4596,8 +4596,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4613,8 +4613,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4630,8 +4630,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4644,10 +4644,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4694,72 +4694,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4834,60 +4834,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4896,10 +4896,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4914,10 +4914,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4933,10 +4933,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4952,10 +4952,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4971,8 +4971,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4988,8 +4988,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5005,8 +5005,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5019,10 +5019,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5069,72 +5069,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5162,16 +5162,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5184,24 +5192,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5226,64 +5226,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5294,8 +5294,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5306,8 +5306,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5318,8 +5318,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5330,8 +5330,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5342,8 +5342,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5354,8 +5354,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5365,8 +5365,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5410,52 +5410,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5465,9 +5465,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5554,60 +5554,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5618,10 +5618,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5636,10 +5636,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5655,10 +5655,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5674,10 +5674,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5693,8 +5693,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5710,8 +5710,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5727,10 +5727,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5793,58 +5793,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5854,12 +5854,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5872,32 +5898,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5923,177 +5923,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6104,10 +6104,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6122,8 +6122,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6139,10 +6139,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6158,8 +6158,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6175,10 +6175,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6194,8 +6194,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6211,10 +6211,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6277,58 +6277,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6338,12 +6338,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6360,23 +6377,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
30.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/September/Others/Cash.xlsx
+++ b/September/Others/Cash.xlsx
@@ -104,7 +104,7 @@
     <t>Rahinul Islam</t>
   </si>
   <si>
-    <t>Date: 29.09.19</t>
+    <t>Date: 30.09.19</t>
   </si>
 </sst>
 </file>
@@ -491,83 +491,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -582,15 +585,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,6 +598,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,12 +625,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,60 +2095,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2157,10 +2157,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2175,10 +2175,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2194,10 +2194,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2213,10 +2213,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2232,10 +2232,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2251,8 +2251,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2268,8 +2268,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2282,10 +2282,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2332,58 +2332,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2393,11 +2393,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2472,60 +2472,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2534,10 +2534,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2552,10 +2552,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2571,10 +2571,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2590,10 +2590,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2609,10 +2609,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2628,8 +2628,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2645,8 +2645,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2659,10 +2659,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2709,58 +2709,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2770,11 +2770,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2802,14 +2802,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2822,24 +2832,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2870,63 +2870,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2936,10 +2936,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2954,13 +2954,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>103</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>26</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>103000</v>
+        <v>26000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>228</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>275</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>114000</v>
+        <v>137500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>262</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>435</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>26200</v>
+        <v>43500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>27</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>29</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>1350</v>
+        <v>1450</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3030,13 +3030,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>10</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>45</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>900</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3049,13 +3049,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58">
-        <v>125</v>
-      </c>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53">
+        <v>65</v>
+      </c>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1250</v>
+        <v>650</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3065,14 +3065,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>246000</v>
+        <v>210000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3124,35 +3124,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3164,9 +3164,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3176,9 +3176,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3265,60 +3265,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3327,10 +3327,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3345,13 +3345,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>103</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>26</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>103000</v>
+        <v>26000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3364,13 +3364,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>228</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>275</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>114000</v>
+        <v>137500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3383,13 +3383,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>262</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>435</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>26200</v>
+        <v>43500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3402,13 +3402,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>27</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>29</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>1350</v>
+        <v>1450</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3421,13 +3421,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>10</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>45</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>200</v>
+        <v>900</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3440,13 +3440,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58">
-        <v>125</v>
-      </c>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53">
+        <v>65</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1250</v>
+        <v>650</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3456,14 +3456,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>246000</v>
+        <v>210000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3515,35 +3515,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3555,9 +3555,9 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3567,9 +3567,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3597,26 +3597,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3631,6 +3611,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3661,63 +3661,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3727,10 +3727,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3745,10 +3745,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3764,10 +3764,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3783,10 +3783,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3802,10 +3802,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3821,10 +3821,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3840,8 +3840,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3854,10 +3854,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3904,76 +3904,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4048,60 +4048,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4110,10 +4110,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4128,10 +4128,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4147,10 +4147,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4166,10 +4166,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4185,10 +4185,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4204,10 +4204,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4223,8 +4223,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4237,10 +4237,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4287,76 +4287,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4384,30 +4384,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4424,6 +4400,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4455,63 +4455,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4521,10 +4521,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4539,10 +4539,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4558,10 +4558,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4577,10 +4577,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4596,8 +4596,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4613,8 +4613,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4630,8 +4630,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4644,10 +4644,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4694,72 +4694,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4834,60 +4834,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4896,10 +4896,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4914,10 +4914,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4933,10 +4933,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4952,10 +4952,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4971,8 +4971,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4988,8 +4988,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5005,8 +5005,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5019,10 +5019,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5069,72 +5069,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5162,6 +5162,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5174,34 +5202,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5226,64 +5226,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5294,8 +5294,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/